<commit_message>
Update Versions of Sprint Backlog and Burndown Chart
Author: Team member 56971
Description: Updated the sprint backlog file and the burndown chart file to its most recent versions
</commit_message>
<xml_diff>
--- a/Project/Phase 1/Sprint 2/Sprint 2 Backlog.xlsx
+++ b/Project/Phase 1/Sprint 2/Sprint 2 Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaov\Downloads\EstudoDT\3ºano\ES\Sprint 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0552EE-3CE7-44F6-BF1D-A7E9B89D28D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA83F4E-7370-4A49-B622-D2A604D3F8C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
   <si>
     <t>Task</t>
   </si>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t>Design Pattern 9</t>
-  </si>
-  <si>
-    <t>To do</t>
   </si>
   <si>
     <t>Gonçalo Virgínia</t>
@@ -165,7 +162,192 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="65">
+  <dxfs count="85">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1047,7 +1229,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,10 +1253,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
         <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1082,10 +1264,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1093,10 +1275,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1104,10 +1286,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1115,65 +1297,65 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
         <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1181,10 +1363,10 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1192,10 +1374,10 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1203,10 +1385,10 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1217,7 +1399,7 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1225,10 +1407,10 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1236,10 +1418,10 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1247,10 +1429,10 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1258,10 +1440,10 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1272,238 +1454,294 @@
         <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D1">
-    <cfRule type="containsText" dxfId="64" priority="77" operator="containsText" text="To do">
+    <cfRule type="containsText" dxfId="84" priority="113" operator="containsText" text="To do">
       <formula>NOT(ISERROR(SEARCH("To do",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A12:C14 F5:XFD9 A30:XFD1048576 A27:I29 E15:I26 N15:XFD29 D12:D18 D11:XFD14 E10:XFD10 D7:D9 C7:C11 D21:D26 C15:C18 A15:A20 C19:D20 A5:A11 A1:XFD4 C5:D6">
-    <cfRule type="containsText" dxfId="63" priority="73" operator="containsText" text="Done">
+  <conditionalFormatting sqref="F5:XFD9 A30:XFD1048576 A27:I29 E15:I26 N15:XFD29 D12:D18 D11:XFD14 E10:XFD10 D7:D9 D21:D26 C19:D20 A1:XFD1 C5:D6 A5:A20 C7:C18 A3:XFD4 A2 C2:XFD2">
+    <cfRule type="containsText" dxfId="83" priority="109" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="74" operator="containsText" text="Reviewing">
+    <cfRule type="containsText" dxfId="82" priority="110" operator="containsText" text="Reviewing">
       <formula>NOT(ISERROR(SEARCH("Reviewing",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="75" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="81" priority="111" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="76" operator="containsText" text="To do">
+    <cfRule type="containsText" dxfId="80" priority="112" operator="containsText" text="To do">
       <formula>NOT(ISERROR(SEARCH("To do",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A21:A26 C21:C26">
+    <cfRule type="containsText" dxfId="79" priority="97" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",A21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="78" priority="98" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",A21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="77" priority="99" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",A21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="76" priority="100" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",A21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11">
+    <cfRule type="containsText" dxfId="75" priority="93" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="74" priority="94" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="73" priority="95" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="72" priority="96" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21:B26">
+    <cfRule type="containsText" dxfId="71" priority="81" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="70" priority="82" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="69" priority="83" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="68" priority="84" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16">
+    <cfRule type="containsText" dxfId="67" priority="73" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="66" priority="74" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="65" priority="75" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="76" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17">
+    <cfRule type="containsText" dxfId="63" priority="69" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="62" priority="70" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="61" priority="71" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="60" priority="72" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="containsText" dxfId="59" priority="65" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="58" priority="66" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="57" priority="67" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="56" priority="68" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18">
+    <cfRule type="containsText" dxfId="55" priority="57" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="54" priority="58" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="53" priority="59" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="60" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="containsText" dxfId="47" priority="45" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="46" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="45" priority="47" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="48" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="containsText" dxfId="43" priority="41" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="42" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="43" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="44" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="containsText" dxfId="39" priority="37" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="38" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="39" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="40" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14">
+    <cfRule type="containsText" dxfId="35" priority="33" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="34" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="35" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="36" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13">
+    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12">
+    <cfRule type="containsText" dxfId="27" priority="25" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="26" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="containsText" dxfId="59" priority="69" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="23" priority="21" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="70" operator="containsText" text="Reviewing">
+    <cfRule type="containsText" dxfId="22" priority="22" operator="containsText" text="Reviewing">
       <formula>NOT(ISERROR(SEARCH("Reviewing",B10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="71" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="21" priority="23" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",B10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="72" operator="containsText" text="To do">
+    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="To do">
       <formula>NOT(ISERROR(SEARCH("To do",B10)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A21:A26 C21:C26">
-    <cfRule type="containsText" dxfId="55" priority="61" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="62" operator="containsText" text="Reviewing">
-      <formula>NOT(ISERROR(SEARCH("Reviewing",A21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="63" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",A21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="64" operator="containsText" text="To do">
-      <formula>NOT(ISERROR(SEARCH("To do",A21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B11">
-    <cfRule type="containsText" dxfId="51" priority="57" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",B11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="58" operator="containsText" text="Reviewing">
-      <formula>NOT(ISERROR(SEARCH("Reviewing",B11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="59" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",B11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="60" operator="containsText" text="To do">
-      <formula>NOT(ISERROR(SEARCH("To do",B11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21:B26">
-    <cfRule type="containsText" dxfId="47" priority="45" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",B21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="46" operator="containsText" text="Reviewing">
-      <formula>NOT(ISERROR(SEARCH("Reviewing",B21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="47" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",B21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="48" operator="containsText" text="To do">
-      <formula>NOT(ISERROR(SEARCH("To do",B21)))</formula>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="43" priority="41" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="42" operator="containsText" text="Reviewing">
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="Reviewing">
       <formula>NOT(ISERROR(SEARCH("Reviewing",B15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="43" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",B15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="44" operator="containsText" text="To do">
+    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="To do">
       <formula>NOT(ISERROR(SEARCH("To do",B15)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16">
-    <cfRule type="containsText" dxfId="39" priority="37" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",B16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="38" operator="containsText" text="Reviewing">
-      <formula>NOT(ISERROR(SEARCH("Reviewing",B16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="39" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",B16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="40" operator="containsText" text="To do">
-      <formula>NOT(ISERROR(SEARCH("To do",B16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17">
-    <cfRule type="containsText" dxfId="35" priority="33" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",B17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="34" operator="containsText" text="Reviewing">
-      <formula>NOT(ISERROR(SEARCH("Reviewing",B17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="35" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",B17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="36" operator="containsText" text="To do">
-      <formula>NOT(ISERROR(SEARCH("To do",B17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19">
-    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",B19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="Reviewing">
-      <formula>NOT(ISERROR(SEARCH("Reviewing",B19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",B19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="To do">
-      <formula>NOT(ISERROR(SEARCH("To do",B19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="containsText" dxfId="27" priority="25" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="26" operator="containsText" text="Reviewing">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Reviewing">
       <formula>NOT(ISERROR(SEARCH("Reviewing",B20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",B20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="To do">
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="To do">
       <formula>NOT(ISERROR(SEARCH("To do",B20)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B18">
-    <cfRule type="containsText" dxfId="23" priority="21" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",B18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="22" operator="containsText" text="Reviewing">
-      <formula>NOT(ISERROR(SEARCH("Reviewing",B18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="23" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",B18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="To do">
-      <formula>NOT(ISERROR(SEARCH("To do",B18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9">
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",B9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Reviewing">
-      <formula>NOT(ISERROR(SEARCH("Reviewing",B9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",B9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="To do">
-      <formula>NOT(ISERROR(SEARCH("To do",B9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="Reviewing">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Reviewing">
       <formula>NOT(ISERROR(SEARCH("Reviewing",B8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",B8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="To do">
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="To do">
       <formula>NOT(ISERROR(SEARCH("To do",B8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",B7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="Reviewing">
-      <formula>NOT(ISERROR(SEARCH("Reviewing",B7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",B7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="To do">
-      <formula>NOT(ISERROR(SEARCH("To do",B7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",B6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Reviewing">
-      <formula>NOT(ISERROR(SEARCH("Reviewing",B6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",B6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="To do">
-      <formula>NOT(ISERROR(SEARCH("To do",B6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",B5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Reviewing">
-      <formula>NOT(ISERROR(SEARCH("Reviewing",B5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",B5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="To do">
-      <formula>NOT(ISERROR(SEARCH("To do",B5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated the sprint backlog and burndow chart
Author: João Vieira 56971
Description: Uploaded the most current version of the sprint backlog file and the burndown chart file
</commit_message>
<xml_diff>
--- a/Project/Phase 1/Sprint 2/Sprint 2 Backlog.xlsx
+++ b/Project/Phase 1/Sprint 2/Sprint 2 Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaov\Downloads\EstudoDT\3ºano\ES\Sprint 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA83F4E-7370-4A49-B622-D2A604D3F8C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA9CFBA-6EC2-46FC-84EF-75AEEB63620D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
   <si>
     <t>Task</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>Guilherme Pereira</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>Metrics 1</t>
@@ -162,7 +159,229 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="85">
+  <dxfs count="109">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1229,7 +1448,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,7 +1472,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -1264,7 +1483,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -1275,7 +1494,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
@@ -1286,7 +1505,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
@@ -1297,7 +1516,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
@@ -1305,10 +1524,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
@@ -1316,10 +1535,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -1327,10 +1546,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
@@ -1338,10 +1557,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
@@ -1349,10 +1568,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
@@ -1396,7 +1615,7 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
@@ -1418,7 +1637,7 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
@@ -1429,7 +1648,7 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
         <v>19</v>
@@ -1440,7 +1659,7 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
         <v>19</v>
@@ -1451,7 +1670,7 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
         <v>19</v>
@@ -1460,288 +1679,316 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D1">
-    <cfRule type="containsText" dxfId="84" priority="113" operator="containsText" text="To do">
+    <cfRule type="containsText" dxfId="108" priority="149" operator="containsText" text="To do">
       <formula>NOT(ISERROR(SEARCH("To do",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F5:XFD9 A30:XFD1048576 A27:I29 E15:I26 N15:XFD29 D12:D18 D11:XFD14 E10:XFD10 D7:D9 D21:D26 C19:D20 A1:XFD1 C5:D6 A5:A20 C7:C18 A3:XFD4 A2 C2:XFD2">
-    <cfRule type="containsText" dxfId="83" priority="109" operator="containsText" text="Done">
+  <conditionalFormatting sqref="F5:XFD9 A30:XFD1048576 A27:I29 E15:I26 N15:XFD29 D12:D18 D11:XFD14 E10:XFD10 D7:D9 D21:D26 C19:D20 A1:XFD1 C5:D6 C7:C18 A2:A20 C2:XFD4">
+    <cfRule type="containsText" dxfId="107" priority="145" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="110" operator="containsText" text="Reviewing">
+    <cfRule type="containsText" dxfId="106" priority="146" operator="containsText" text="Reviewing">
       <formula>NOT(ISERROR(SEARCH("Reviewing",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="111" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="105" priority="147" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="112" operator="containsText" text="To do">
+    <cfRule type="containsText" dxfId="104" priority="148" operator="containsText" text="To do">
       <formula>NOT(ISERROR(SEARCH("To do",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:A26 C21:C26">
-    <cfRule type="containsText" dxfId="79" priority="97" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="103" priority="133" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="98" operator="containsText" text="Reviewing">
+    <cfRule type="containsText" dxfId="102" priority="134" operator="containsText" text="Reviewing">
       <formula>NOT(ISERROR(SEARCH("Reviewing",A21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="99" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="101" priority="135" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",A21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="100" operator="containsText" text="To do">
+    <cfRule type="containsText" dxfId="100" priority="136" operator="containsText" text="To do">
       <formula>NOT(ISERROR(SEARCH("To do",A21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="containsText" dxfId="75" priority="93" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="99" priority="129" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="94" operator="containsText" text="Reviewing">
+    <cfRule type="containsText" dxfId="98" priority="130" operator="containsText" text="Reviewing">
       <formula>NOT(ISERROR(SEARCH("Reviewing",B11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="95" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="97" priority="131" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",B11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="96" operator="containsText" text="To do">
+    <cfRule type="containsText" dxfId="96" priority="132" operator="containsText" text="To do">
       <formula>NOT(ISERROR(SEARCH("To do",B11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:B26">
-    <cfRule type="containsText" dxfId="71" priority="81" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="95" priority="117" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="82" operator="containsText" text="Reviewing">
+    <cfRule type="containsText" dxfId="94" priority="118" operator="containsText" text="Reviewing">
       <formula>NOT(ISERROR(SEARCH("Reviewing",B21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="83" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="93" priority="119" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",B21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="84" operator="containsText" text="To do">
+    <cfRule type="containsText" dxfId="92" priority="120" operator="containsText" text="To do">
       <formula>NOT(ISERROR(SEARCH("To do",B21)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B17">
+    <cfRule type="containsText" dxfId="91" priority="105" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="90" priority="106" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="89" priority="107" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="88" priority="108" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="containsText" dxfId="87" priority="101" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="86" priority="102" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="85" priority="103" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="84" priority="104" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18">
+    <cfRule type="containsText" dxfId="83" priority="93" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="82" priority="94" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="81" priority="95" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="80" priority="96" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="containsText" dxfId="79" priority="81" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="78" priority="82" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="77" priority="83" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="76" priority="84" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="containsText" dxfId="75" priority="77" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="74" priority="78" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="73" priority="79" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="72" priority="80" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="containsText" dxfId="71" priority="73" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="70" priority="74" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="69" priority="75" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="68" priority="76" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15">
+    <cfRule type="containsText" dxfId="55" priority="45" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="54" priority="46" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="53" priority="47" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="48" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20">
+    <cfRule type="containsText" dxfId="51" priority="41" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="50" priority="42" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="43" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="48" priority="44" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="containsText" dxfId="47" priority="37" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="38" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="45" priority="39" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="40" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="containsText" dxfId="67" priority="73" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="43" priority="33" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="74" operator="containsText" text="Reviewing">
+    <cfRule type="containsText" dxfId="42" priority="34" operator="containsText" text="Reviewing">
       <formula>NOT(ISERROR(SEARCH("Reviewing",B16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="75" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="41" priority="35" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",B16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="76" operator="containsText" text="To do">
+    <cfRule type="containsText" dxfId="40" priority="36" operator="containsText" text="To do">
       <formula>NOT(ISERROR(SEARCH("To do",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17">
-    <cfRule type="containsText" dxfId="63" priority="69" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",B17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="70" operator="containsText" text="Reviewing">
-      <formula>NOT(ISERROR(SEARCH("Reviewing",B17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="71" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",B17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="72" operator="containsText" text="To do">
-      <formula>NOT(ISERROR(SEARCH("To do",B17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19">
-    <cfRule type="containsText" dxfId="59" priority="65" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",B19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="66" operator="containsText" text="Reviewing">
-      <formula>NOT(ISERROR(SEARCH("Reviewing",B19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="67" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",B19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="68" operator="containsText" text="To do">
-      <formula>NOT(ISERROR(SEARCH("To do",B19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18">
-    <cfRule type="containsText" dxfId="55" priority="57" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",B18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="58" operator="containsText" text="Reviewing">
-      <formula>NOT(ISERROR(SEARCH("Reviewing",B18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="59" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",B18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="60" operator="containsText" text="To do">
-      <formula>NOT(ISERROR(SEARCH("To do",B18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
-    <cfRule type="containsText" dxfId="47" priority="45" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",B7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="46" operator="containsText" text="Reviewing">
-      <formula>NOT(ISERROR(SEARCH("Reviewing",B7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="47" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",B7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="48" operator="containsText" text="To do">
-      <formula>NOT(ISERROR(SEARCH("To do",B7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6">
-    <cfRule type="containsText" dxfId="43" priority="41" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",B6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="42" operator="containsText" text="Reviewing">
-      <formula>NOT(ISERROR(SEARCH("Reviewing",B6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="43" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",B6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="44" operator="containsText" text="To do">
-      <formula>NOT(ISERROR(SEARCH("To do",B6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5">
-    <cfRule type="containsText" dxfId="39" priority="37" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",B5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="38" operator="containsText" text="Reviewing">
-      <formula>NOT(ISERROR(SEARCH("Reviewing",B5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="39" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",B5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="40" operator="containsText" text="To do">
-      <formula>NOT(ISERROR(SEARCH("To do",B5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="containsText" dxfId="35" priority="33" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="39" priority="29" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="34" operator="containsText" text="Reviewing">
+    <cfRule type="containsText" dxfId="38" priority="30" operator="containsText" text="Reviewing">
       <formula>NOT(ISERROR(SEARCH("Reviewing",B14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="35" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="37" priority="31" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",B14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="36" operator="containsText" text="To do">
+    <cfRule type="containsText" dxfId="36" priority="32" operator="containsText" text="To do">
       <formula>NOT(ISERROR(SEARCH("To do",B14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="35" priority="25" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="Reviewing">
+    <cfRule type="containsText" dxfId="34" priority="26" operator="containsText" text="Reviewing">
       <formula>NOT(ISERROR(SEARCH("Reviewing",B13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="33" priority="27" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",B13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="To do">
+    <cfRule type="containsText" dxfId="32" priority="28" operator="containsText" text="To do">
       <formula>NOT(ISERROR(SEARCH("To do",B13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="containsText" dxfId="27" priority="25" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="31" priority="21" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="26" operator="containsText" text="Reviewing">
+    <cfRule type="containsText" dxfId="30" priority="22" operator="containsText" text="Reviewing">
       <formula>NOT(ISERROR(SEARCH("Reviewing",B12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="29" priority="23" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",B12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="To do">
+    <cfRule type="containsText" dxfId="28" priority="24" operator="containsText" text="To do">
       <formula>NOT(ISERROR(SEARCH("To do",B12)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="containsText" dxfId="27" priority="17" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="18" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="19" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="20" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="containsText" dxfId="23" priority="13" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="14" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="15" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="containsText" dxfId="19" priority="9" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="10" operator="containsText" text="Reviewing">
+      <formula>NOT(ISERROR(SEARCH("Reviewing",B9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="11" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="12" operator="containsText" text="To do">
+      <formula>NOT(ISERROR(SEARCH("To do",B9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="containsText" dxfId="23" priority="21" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="22" operator="containsText" text="Reviewing">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Reviewing">
       <formula>NOT(ISERROR(SEARCH("Reviewing",B10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="23" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",B10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="To do">
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="To do">
       <formula>NOT(ISERROR(SEARCH("To do",B10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Reviewing">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Reviewing">
       <formula>NOT(ISERROR(SEARCH("Reviewing",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="To do">
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="To do">
       <formula>NOT(ISERROR(SEARCH("To do",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9">
-    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",B9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="Reviewing">
-      <formula>NOT(ISERROR(SEARCH("Reviewing",B9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",B9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="To do">
-      <formula>NOT(ISERROR(SEARCH("To do",B9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",B15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="Reviewing">
-      <formula>NOT(ISERROR(SEARCH("Reviewing",B15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",B15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="To do">
-      <formula>NOT(ISERROR(SEARCH("To do",B15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B20">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",B20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Reviewing">
-      <formula>NOT(ISERROR(SEARCH("Reviewing",B20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",B20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="To do">
-      <formula>NOT(ISERROR(SEARCH("To do",B20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",B8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Reviewing">
-      <formula>NOT(ISERROR(SEARCH("Reviewing",B8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",B8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="To do">
-      <formula>NOT(ISERROR(SEARCH("To do",B8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>